<commit_message>
Cập nhật biên bản họp, báo cáo, link video họp
</commit_message>
<xml_diff>
--- a/Report/230321_FIT_LinkVideo_Nhom4.xlsx
+++ b/Report/230321_FIT_LinkVideo_Nhom4.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TTCSN_Group5_HAUI\Biên bản, báo cáo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TTCSN_Group5_HAUI\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7F572F-43CB-4D4F-A09B-0E842F155C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11F9B3B-FDE3-44D1-AC5D-9A0503EA6D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
+    <sheet name="LinkVideoHop" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Buổi họp Kickkoff (14/03/2023)</t>
   </si>
@@ -81,12 +81,18 @@
   <si>
     <t>https://drive.google.com/file/d/1W0R2QY9llidZTmqYfW7mp8WTCKySuseq/view?usp=share_link</t>
   </si>
+  <si>
+    <t>https://drive.google.com/file/d/1X8LjLjhU_040XppXpnyKggoh4SRC1vYG/view?usp=share_link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video họp tuần 11 (27/05/2023) </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -116,6 +122,26 @@
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -134,10 +160,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -145,8 +172,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -363,10 +393,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="24.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -696,8 +726,12 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="24.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -28387,34 +28421,6 @@
       <c r="Y999" s="1"/>
       <c r="Z999" s="1"/>
     </row>
-    <row r="1000" spans="1:26" ht="24.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1000" s="1"/>
-      <c r="B1000" s="1"/>
-      <c r="C1000" s="1"/>
-      <c r="D1000" s="1"/>
-      <c r="E1000" s="1"/>
-      <c r="F1000" s="1"/>
-      <c r="G1000" s="1"/>
-      <c r="H1000" s="1"/>
-      <c r="I1000" s="1"/>
-      <c r="J1000" s="1"/>
-      <c r="K1000" s="1"/>
-      <c r="L1000" s="1"/>
-      <c r="M1000" s="1"/>
-      <c r="N1000" s="1"/>
-      <c r="O1000" s="1"/>
-      <c r="P1000" s="1"/>
-      <c r="Q1000" s="1"/>
-      <c r="R1000" s="1"/>
-      <c r="S1000" s="1"/>
-      <c r="T1000" s="1"/>
-      <c r="U1000" s="1"/>
-      <c r="V1000" s="1"/>
-      <c r="W1000" s="1"/>
-      <c r="X1000" s="1"/>
-      <c r="Y1000" s="1"/>
-      <c r="Z1000" s="1"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -28427,7 +28433,9 @@
     <hyperlink ref="B8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="B9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="B10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B11" r:id="rId11" xr:uid="{4683D3A5-6EA3-4000-B4F1-E021A808878E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>